<commit_message>
major_update: pc portátil hp
</commit_message>
<xml_diff>
--- a/2. Hardware PCB/REV_4.0/measurement/Project Outputs for measurement_rev4/Pick Place for measurement_rev4.xlsx
+++ b/2. Hardware PCB/REV_4.0/measurement/Project Outputs for measurement_rev4/Pick Place for measurement_rev4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\20190909 - 3phase_inverter\3phase_inverter\2. Hardware PCB\REV_4.0\measurement\Project Outputs for measurement_rev4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VMORAIS\Desktop\3phase_inverter\2. Hardware PCB\REV_4.0\measurement\Project Outputs for measurement_rev4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,12 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="164">
   <si>
     <t>Altium Designer Pick and Place Locations</t>
   </si>
   <si>
-    <t>F:\Projects\20190909 - 3phase_inverter\3phase_inverter\2. Hardware PCB\REV_4.0\measurement\Project Outputs for measurement_rev4\Pick Place for measurement_rev4.csv</t>
+    <t>C:\Users\VMORAIS\Desktop\3phase_inverter\2. Hardware PCB\REV_4.0\measurement\Project Outputs for measurement_rev4\Pick Place for measurement_rev4.csv</t>
   </si>
   <si>
     <t>========================================================================================================================</t>
@@ -33,10 +33,10 @@
     <t>File Design Information:</t>
   </si>
   <si>
-    <t>Date:       11/03/20</t>
-  </si>
-  <si>
-    <t>Time:       17:58</t>
+    <t>Date:       15/03/20</t>
+  </si>
+  <si>
+    <t>Time:       15:06</t>
   </si>
   <si>
     <t>Revision:   Not in VersionControl</t>
@@ -75,376 +75,442 @@
     <t>LCSC PART #</t>
   </si>
   <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P 8p 2.54 SR DW 8P</t>
+  </si>
+  <si>
+    <t>TopLayer</t>
+  </si>
+  <si>
+    <t>Header_8x1_8.5mm</t>
+  </si>
+  <si>
+    <t>Distribuidores e Alojamento de Fios CGrid Hrd SRDW THo le 8ckt</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>P 2p 5mm</t>
+  </si>
+  <si>
+    <t>BottomLayer</t>
+  </si>
+  <si>
+    <t>connector1x2_parafuso</t>
+  </si>
+  <si>
+    <t>Bloques de terminales de PCB de perfil estándar RS de 5,0 mm</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>CC3</t>
+  </si>
+  <si>
+    <t>IC CC 30A SO-8</t>
+  </si>
+  <si>
+    <t>CC6303_SOP8</t>
+  </si>
+  <si>
+    <t>Sensores de Corrente de Montagem de Painel Hall Effect IC LF 30A 66 mV/A</t>
+  </si>
+  <si>
+    <t>C10681</t>
+  </si>
+  <si>
+    <t>CC2</t>
+  </si>
+  <si>
+    <t>CC1</t>
+  </si>
+  <si>
+    <t>XMC1</t>
+  </si>
+  <si>
+    <t>IC XMC4500 Relax LITE</t>
+  </si>
+  <si>
+    <t>XMC4500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  KIT_XMC45_RELAX_LITE_V1 -  Evaluation Board</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> XMC4500 MCU</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Detachable On-Board Debugger</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> USB Powered ""</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R 7k5 1/8W 0805 .1%</t>
+  </si>
+  <si>
+    <t>RESC_0805</t>
+  </si>
+  <si>
+    <t>Resistores de Filme Fino - SMD 7.5K OHM .1% 25ppm</t>
+  </si>
+  <si>
+    <t>C17807</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>R 5k1 1/8W 0805 .1%</t>
+  </si>
+  <si>
+    <t>Resistores de Filme Fino - SMD 0805 5.1Kohm 1/8W .1% 25ppm</t>
+  </si>
+  <si>
+    <t>C27834</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>U12</t>
+  </si>
+  <si>
+    <t>IC CC/CC 1W 5V</t>
+  </si>
+  <si>
+    <t>DC/DC_ISO</t>
+  </si>
+  <si>
+    <t>Conversores CC/CC com isolação 1W 5Vin 5Vout 200mA SIP7</t>
+  </si>
+  <si>
+    <t>U13</t>
+  </si>
+  <si>
+    <t>IC AmpIso BIPOL AMC1200</t>
+  </si>
+  <si>
+    <t>SOIC8</t>
+  </si>
+  <si>
+    <t>Amplificadores de isolamento 4kV peak Iso Amp</t>
+  </si>
+  <si>
+    <t>C79905</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R 560 1/8W 0805 .1%</t>
+  </si>
+  <si>
+    <t>Resistores de Filme Fino - SMD 1/8W 3.6K ohm .1% 25ppm</t>
+  </si>
+  <si>
+    <t>C28636</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R 330 1/8 0805 .1%</t>
+  </si>
+  <si>
+    <t>Resistores de Filme Fino - SMD CPF 0805 330R 0.1% 25PPM 1K RL</t>
+  </si>
+  <si>
+    <t>C17630</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R 100k 1/8W 0805 .1%</t>
+  </si>
+  <si>
+    <t>Resistores de Filme Fino - SMD 100 Kohm .1% 0805 25PPM</t>
+  </si>
+  <si>
+    <t>C17407</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>R19</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C 10uF 0805 MLCC 25V X5R</t>
+  </si>
+  <si>
+    <t>CAPC_0805</t>
+  </si>
+  <si>
+    <t>Capacitores de cerâmica multicamada MLCC - SMD/SMT 10uF 25V X5R +/-10% 0805 Gen Purp</t>
+  </si>
+  <si>
+    <t>C15850</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C 1uF 0805 MLCC 50V X5R</t>
+  </si>
+  <si>
+    <t>Capacitores de cerâmica multicamada MLCC - SMD/SMT 0805 50V 1uF 20% X5R</t>
+  </si>
+  <si>
+    <t>C28323</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C 10nF 0805 MLCC 50V X7R</t>
+  </si>
+  <si>
+    <t>Capacitores de cerâmica multicamada MLCC - SMD/SMT 10nF 50V X7R 10%</t>
+  </si>
+  <si>
+    <t>C1710</t>
+  </si>
+  <si>
+    <t>U15</t>
+  </si>
+  <si>
+    <t>R44</t>
+  </si>
+  <si>
+    <t>R43</t>
+  </si>
+  <si>
+    <t>R42</t>
+  </si>
+  <si>
+    <t>R41</t>
+  </si>
+  <si>
+    <t>R40</t>
+  </si>
+  <si>
+    <t>R34</t>
+  </si>
+  <si>
+    <t>R33</t>
+  </si>
+  <si>
+    <t>R32</t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>R35</t>
+  </si>
+  <si>
+    <t>R36</t>
+  </si>
+  <si>
+    <t>R37</t>
+  </si>
+  <si>
+    <t>R38</t>
+  </si>
+  <si>
+    <t>R39</t>
+  </si>
+  <si>
+    <t>U14</t>
+  </si>
+  <si>
+    <t>U16</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>U17</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R 10 1/8W 0805 1%</t>
+  </si>
+  <si>
+    <t>Resistores de Filme Espesso - SMD 1/8Watt 10ohms 1% Commercial Use</t>
+  </si>
+  <si>
+    <t>C17415</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>U10</t>
+  </si>
+  <si>
+    <t>IC Relay 5A 5V 5x20mm</t>
+  </si>
+  <si>
+    <t>Relay_-_G6DN</t>
+  </si>
+  <si>
+    <t>Relés para uso geral 1 form A w/ 5VDC Coil-standard type</t>
+  </si>
+  <si>
+    <t>U11</t>
+  </si>
+  <si>
     <t>U6</t>
   </si>
   <si>
-    <t>P 2p 5mm</t>
-  </si>
-  <si>
-    <t>BottomLayer</t>
-  </si>
-  <si>
-    <t>connector1x2_parafuso</t>
-  </si>
-  <si>
-    <t>Bloques de terminales de PCB de perfil estándar RS de 5,0 mm</t>
+    <t>IC DUAL MOS DRIVER MIC4127</t>
+  </si>
+  <si>
+    <t>SOIC-MIC4126</t>
+  </si>
+  <si>
+    <t>Drivers de portas 1.5A Dual High Speed MOSFET Driver with Low Thermal Impedance</t>
+  </si>
+  <si>
+    <t>C18690</t>
+  </si>
+  <si>
+    <t>U1</t>
   </si>
   <si>
     <t>U5</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>CC3</t>
-  </si>
-  <si>
-    <t>IC CC 30A SO-8</t>
-  </si>
-  <si>
-    <t>TopLayer</t>
-  </si>
-  <si>
-    <t>CC6303_SOP8</t>
-  </si>
-  <si>
-    <t>Sensores de Corrente de Montagem de Painel Hall Effect IC LF 30A 66 mV/A</t>
-  </si>
-  <si>
-    <t>C10681</t>
-  </si>
-  <si>
-    <t>CC2</t>
-  </si>
-  <si>
-    <t>CC1</t>
-  </si>
-  <si>
-    <t>XMC1</t>
-  </si>
-  <si>
-    <t>IC XMC4500 Relax LITE</t>
-  </si>
-  <si>
-    <t>XMC4500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  KIT_XMC45_RELAX_LITE_V1 -  Evaluation Board</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> XMC4500 MCU</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Detachable On-Board Debugger</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> USB Powered ""</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>R 7k5 1/8W 0805 .1%</t>
-  </si>
-  <si>
-    <t>RESC_0805</t>
-  </si>
-  <si>
-    <t>Resistores de Filme Fino - SMD 7.5K OHM .1% 25ppm</t>
-  </si>
-  <si>
-    <t>C17807</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>R 5k1 1/8W 0805 .1%</t>
-  </si>
-  <si>
-    <t>Resistores de Filme Fino - SMD 0805 5.1Kohm 1/8W .1% 25ppm</t>
-  </si>
-  <si>
-    <t>C27834</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>U7</t>
-  </si>
-  <si>
-    <t>IC CC/CC 1W 5V</t>
-  </si>
-  <si>
-    <t>DC/DC_ISO</t>
-  </si>
-  <si>
-    <t>Conversores CC/CC com isolação 1W 5Vin 5Vout 200mA SIP7</t>
-  </si>
-  <si>
-    <t>U8</t>
-  </si>
-  <si>
-    <t>IC AmpIso BIPOL AMC1200</t>
-  </si>
-  <si>
-    <t>SOIC8</t>
-  </si>
-  <si>
-    <t>Amplificadores de isolamento 4kV peak Iso Amp</t>
-  </si>
-  <si>
-    <t>C79905</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>R 560 1/8W 0805 .1%</t>
-  </si>
-  <si>
-    <t>Resistores de Filme Fino - SMD 1/8W 3.6K ohm .1% 25ppm</t>
-  </si>
-  <si>
-    <t>C28636</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>R 330 1/8 0805 .1%</t>
-  </si>
-  <si>
-    <t>Resistores de Filme Fino - SMD CPF 0805 330R 0.1% 25PPM 1K RL</t>
-  </si>
-  <si>
-    <t>C17630</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>R 100k 1/8W 0805 .1%</t>
-  </si>
-  <si>
-    <t>Resistores de Filme Fino - SMD 100 Kohm .1% 0805 25PPM</t>
-  </si>
-  <si>
-    <t>C17407</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>R13</t>
-  </si>
-  <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>R9</t>
-  </si>
-  <si>
-    <t>R18</t>
-  </si>
-  <si>
-    <t>R17</t>
-  </si>
-  <si>
-    <t>R16</t>
-  </si>
-  <si>
-    <t>R15</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C 10uF 0805 MLCC 25V X5R</t>
-  </si>
-  <si>
-    <t>CAPC_0805</t>
-  </si>
-  <si>
-    <t>Capacitores de cerâmica multicamada MLCC - SMD/SMT 10uF 25V X5R +/-10% 0805 Gen Purp</t>
-  </si>
-  <si>
-    <t>C15850</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>C 1uF 0805 MLCC 50V X5R</t>
-  </si>
-  <si>
-    <t>Capacitores de cerâmica multicamada MLCC - SMD/SMT 0805 50V 1uF 20% X5R</t>
-  </si>
-  <si>
-    <t>C28323</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>C 10nF 0805 MLCC 50V X7R</t>
-  </si>
-  <si>
-    <t>Capacitores de cerâmica multicamada MLCC - SMD/SMT 10nF 50V X7R 10%</t>
-  </si>
-  <si>
-    <t>C1710</t>
-  </si>
-  <si>
-    <t>U10</t>
-  </si>
-  <si>
-    <t>R42</t>
-  </si>
-  <si>
-    <t>R41</t>
-  </si>
-  <si>
-    <t>R40</t>
-  </si>
-  <si>
-    <t>R39</t>
-  </si>
-  <si>
-    <t>R38</t>
-  </si>
-  <si>
-    <t>R32</t>
-  </si>
-  <si>
-    <t>R31</t>
-  </si>
-  <si>
-    <t>R30</t>
-  </si>
-  <si>
-    <t>R29</t>
-  </si>
-  <si>
-    <t>R28</t>
-  </si>
-  <si>
-    <t>R22</t>
-  </si>
-  <si>
-    <t>R20</t>
-  </si>
-  <si>
-    <t>C14</t>
-  </si>
-  <si>
-    <t>C13</t>
-  </si>
-  <si>
-    <t>C9</t>
-  </si>
-  <si>
-    <t>C8</t>
-  </si>
-  <si>
-    <t>C6</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>C12</t>
-  </si>
-  <si>
-    <t>C10</t>
-  </si>
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>R19</t>
-  </si>
-  <si>
-    <t>R21</t>
-  </si>
-  <si>
-    <t>R23</t>
-  </si>
-  <si>
-    <t>R24</t>
-  </si>
-  <si>
-    <t>R25</t>
-  </si>
-  <si>
-    <t>R26</t>
-  </si>
-  <si>
-    <t>R27</t>
-  </si>
-  <si>
-    <t>R33</t>
-  </si>
-  <si>
-    <t>R34</t>
-  </si>
-  <si>
-    <t>R35</t>
-  </si>
-  <si>
-    <t>R36</t>
-  </si>
-  <si>
-    <t>R37</t>
-  </si>
-  <si>
-    <t>U9</t>
-  </si>
-  <si>
-    <t>U11</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>P3</t>
-  </si>
-  <si>
-    <t>C15</t>
-  </si>
-  <si>
-    <t>U12</t>
   </si>
 </sst>
 </file>
@@ -1251,15 +1317,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K89"/>
+  <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="J91" sqref="J91"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1350,13 +1418,13 @@
         <v>21</v>
       </c>
       <c r="E14">
-        <v>3627.665</v>
+        <v>1295</v>
       </c>
       <c r="F14">
-        <v>1175</v>
+        <v>3635</v>
       </c>
       <c r="G14">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="H14" t="s">
         <v>22</v>
@@ -1376,13 +1444,13 @@
         <v>21</v>
       </c>
       <c r="E15">
-        <v>3627.6660000000002</v>
+        <v>1295</v>
       </c>
       <c r="F15">
-        <v>2239</v>
+        <v>3735</v>
       </c>
       <c r="G15">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="H15" t="s">
         <v>22</v>
@@ -1393,300 +1461,294 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E16">
         <v>3627.665</v>
       </c>
       <c r="F16">
-        <v>3350</v>
+        <v>1175</v>
       </c>
       <c r="G16">
         <v>90</v>
       </c>
       <c r="H16" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
         <v>25</v>
       </c>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E17">
-        <v>3627.665</v>
+        <v>3627.6660000000002</v>
       </c>
       <c r="F17">
-        <v>685</v>
+        <v>2239</v>
       </c>
       <c r="G17">
         <v>90</v>
       </c>
       <c r="H17" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
         <v>26</v>
       </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E18">
-        <v>3627.6660000000002</v>
+        <v>3627.665</v>
       </c>
       <c r="F18">
-        <v>1750</v>
+        <v>3350</v>
       </c>
       <c r="G18">
         <v>90</v>
       </c>
       <c r="H18" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
         <v>27</v>
       </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" t="s">
-        <v>21</v>
-      </c>
       <c r="E19">
-        <v>3627.6660000000002</v>
+        <v>3627.665</v>
       </c>
       <c r="F19">
-        <v>2860</v>
+        <v>685</v>
       </c>
       <c r="G19">
         <v>90</v>
       </c>
       <c r="H19" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E20">
-        <v>3265</v>
+        <v>3627.6660000000002</v>
       </c>
       <c r="F20">
-        <v>1070</v>
+        <v>1750</v>
       </c>
       <c r="G20">
         <v>90</v>
       </c>
       <c r="H20" t="s">
-        <v>32</v>
-      </c>
-      <c r="I20" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E21">
-        <v>3265</v>
+        <v>3627.6660000000002</v>
       </c>
       <c r="F21">
-        <v>2130</v>
+        <v>2860</v>
       </c>
       <c r="G21">
         <v>90</v>
       </c>
       <c r="H21" t="s">
-        <v>32</v>
-      </c>
-      <c r="I21" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
         <v>35</v>
       </c>
-      <c r="B22" t="s">
-        <v>29</v>
-      </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E22">
         <v>3265</v>
       </c>
       <c r="F22">
-        <v>3245</v>
+        <v>1070</v>
       </c>
       <c r="G22">
         <v>90</v>
       </c>
       <c r="H22" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="I22" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s">
         <v>36</v>
       </c>
-      <c r="B23" t="s">
+      <c r="E23">
+        <v>3265</v>
+      </c>
+      <c r="F23">
+        <v>2130</v>
+      </c>
+      <c r="G23">
+        <v>90</v>
+      </c>
+      <c r="H23" t="s">
         <v>37</v>
       </c>
-      <c r="C23" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="I23" t="s">
         <v>38</v>
-      </c>
-      <c r="E23">
-        <v>1288.5429999999999</v>
-      </c>
-      <c r="F23">
-        <v>2780</v>
-      </c>
-      <c r="G23">
-        <v>360</v>
-      </c>
-      <c r="H23" t="s">
-        <v>39</v>
-      </c>
-      <c r="I23" t="s">
-        <v>40</v>
-      </c>
-      <c r="J23" t="s">
-        <v>41</v>
-      </c>
-      <c r="K23" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E24">
-        <v>2310</v>
+        <v>3265</v>
       </c>
       <c r="F24">
-        <v>1365</v>
+        <v>2875</v>
       </c>
       <c r="G24">
-        <v>270</v>
+        <v>90</v>
       </c>
       <c r="H24" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="I24" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25">
+        <v>1288.5429999999999</v>
+      </c>
+      <c r="F25">
+        <v>2780</v>
+      </c>
+      <c r="G25">
+        <v>360</v>
+      </c>
+      <c r="H25" t="s">
+        <v>44</v>
+      </c>
+      <c r="I25" t="s">
         <v>45</v>
       </c>
-      <c r="E25">
-        <v>2409.8200000000002</v>
-      </c>
-      <c r="F25">
-        <v>1365</v>
-      </c>
-      <c r="G25">
-        <v>90</v>
-      </c>
-      <c r="H25" t="s">
-        <v>50</v>
-      </c>
-      <c r="I25" t="s">
-        <v>51</v>
+      <c r="J25" t="s">
+        <v>46</v>
+      </c>
+      <c r="K25" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E26">
-        <v>615</v>
+        <v>2310</v>
       </c>
       <c r="F26">
         <v>1365</v>
@@ -1695,10 +1757,10 @@
         <v>270</v>
       </c>
       <c r="H26" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I26" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1706,16 +1768,16 @@
         <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D27" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E27">
-        <v>518.33299999999997</v>
+        <v>2409.8200000000002</v>
       </c>
       <c r="F27">
         <v>1365</v>
@@ -1724,27 +1786,27 @@
         <v>90</v>
       </c>
       <c r="H27" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="I27" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D28" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E28">
-        <v>1585</v>
+        <v>615</v>
       </c>
       <c r="F28">
         <v>1365</v>
@@ -1753,27 +1815,27 @@
         <v>270</v>
       </c>
       <c r="H28" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I28" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D29" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E29">
-        <v>1488.3330000000001</v>
+        <v>518.33299999999997</v>
       </c>
       <c r="F29">
         <v>1365</v>
@@ -1782,36 +1844,39 @@
         <v>90</v>
       </c>
       <c r="H29" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="I29" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s">
         <v>20</v>
       </c>
       <c r="D30" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E30">
-        <v>1744.37</v>
+        <v>1585</v>
       </c>
       <c r="F30">
-        <v>965.59100000000001</v>
+        <v>1365</v>
       </c>
       <c r="G30">
         <v>270</v>
       </c>
       <c r="H30" t="s">
-        <v>59</v>
+        <v>51</v>
+      </c>
+      <c r="I30" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1819,144 +1884,141 @@
         <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E31">
-        <v>1370</v>
+        <v>1488.3330000000001</v>
       </c>
       <c r="F31">
-        <v>979.56700000000001</v>
+        <v>1365</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="H31" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="I31" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D32" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="E32">
-        <v>1579.37</v>
+        <v>1744.37</v>
       </c>
       <c r="F32">
-        <v>675</v>
+        <v>965.59100000000001</v>
       </c>
       <c r="G32">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="H32" t="s">
-        <v>67</v>
-      </c>
-      <c r="I32" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33">
+        <v>1370</v>
+      </c>
+      <c r="F33">
+        <v>979.56700000000001</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33" t="s">
+        <v>68</v>
+      </c>
+      <c r="I33" t="s">
         <v>69</v>
-      </c>
-      <c r="B33" t="s">
-        <v>70</v>
-      </c>
-      <c r="C33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D33" t="s">
-        <v>45</v>
-      </c>
-      <c r="E33">
-        <v>1295</v>
-      </c>
-      <c r="F33">
-        <v>1365</v>
-      </c>
-      <c r="G33">
-        <v>90</v>
-      </c>
-      <c r="H33" t="s">
-        <v>71</v>
-      </c>
-      <c r="I33" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E34">
-        <v>1784.37</v>
+        <v>1579.37</v>
       </c>
       <c r="F34">
-        <v>310</v>
+        <v>675</v>
       </c>
       <c r="G34">
         <v>180</v>
       </c>
       <c r="H34" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I34" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35">
+        <v>1295</v>
+      </c>
+      <c r="F35">
+        <v>1365</v>
+      </c>
+      <c r="G35">
+        <v>90</v>
+      </c>
+      <c r="H35" t="s">
+        <v>76</v>
+      </c>
+      <c r="I35" t="s">
         <v>77</v>
-      </c>
-      <c r="B35" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" t="s">
-        <v>30</v>
-      </c>
-      <c r="D35" t="s">
-        <v>45</v>
-      </c>
-      <c r="E35">
-        <v>1784.37</v>
-      </c>
-      <c r="F35">
-        <v>445</v>
-      </c>
-      <c r="G35">
-        <v>360</v>
-      </c>
-      <c r="H35" t="s">
-        <v>75</v>
-      </c>
-      <c r="I35" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1964,312 +2026,312 @@
         <v>78</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C36" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E36">
         <v>1784.37</v>
       </c>
       <c r="F36">
-        <v>580</v>
+        <v>310</v>
       </c>
       <c r="G36">
         <v>180</v>
       </c>
       <c r="H36" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I36" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" t="s">
         <v>79</v>
       </c>
-      <c r="B37" t="s">
-        <v>74</v>
-      </c>
       <c r="C37" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D37" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E37">
-        <v>1921.7719999999999</v>
+        <v>1784.37</v>
       </c>
       <c r="F37">
-        <v>240</v>
+        <v>445</v>
       </c>
       <c r="G37">
-        <v>90</v>
+        <v>360</v>
       </c>
       <c r="H37" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I37" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38">
+        <v>1784.37</v>
+      </c>
+      <c r="F38">
+        <v>580</v>
+      </c>
+      <c r="G38">
+        <v>180</v>
+      </c>
+      <c r="H38" t="s">
         <v>80</v>
       </c>
-      <c r="B38" t="s">
-        <v>74</v>
-      </c>
-      <c r="C38" t="s">
-        <v>30</v>
-      </c>
-      <c r="D38" t="s">
-        <v>45</v>
-      </c>
-      <c r="E38">
-        <v>1884.37</v>
-      </c>
-      <c r="F38">
-        <v>65</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38" t="s">
-        <v>75</v>
-      </c>
       <c r="I38" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39">
+        <v>1921.7719999999999</v>
+      </c>
+      <c r="F39">
+        <v>240</v>
+      </c>
+      <c r="G39">
+        <v>90</v>
+      </c>
+      <c r="H39" t="s">
+        <v>80</v>
+      </c>
+      <c r="I39" t="s">
         <v>81</v>
-      </c>
-      <c r="B39" t="s">
-        <v>74</v>
-      </c>
-      <c r="C39" t="s">
-        <v>30</v>
-      </c>
-      <c r="D39" t="s">
-        <v>45</v>
-      </c>
-      <c r="E39">
-        <v>1385</v>
-      </c>
-      <c r="F39">
-        <v>580</v>
-      </c>
-      <c r="G39">
-        <v>360</v>
-      </c>
-      <c r="H39" t="s">
-        <v>75</v>
-      </c>
-      <c r="I39" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C40" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D40" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E40">
-        <v>1384.37</v>
+        <v>1884.37</v>
       </c>
       <c r="F40">
-        <v>445</v>
+        <v>65</v>
       </c>
       <c r="G40">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="H40" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I40" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B41" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C41" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D41" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E41">
-        <v>1384.37</v>
+        <v>1385</v>
       </c>
       <c r="F41">
-        <v>310</v>
+        <v>580</v>
       </c>
       <c r="G41">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="H41" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I41" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B42" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C42" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D42" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E42">
-        <v>1249.3699999999999</v>
+        <v>1384.37</v>
       </c>
       <c r="F42">
-        <v>240</v>
+        <v>445</v>
       </c>
       <c r="G42">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="H42" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I42" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B43" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C43" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D43" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E43">
-        <v>1289.3699999999999</v>
+        <v>1384.37</v>
       </c>
       <c r="F43">
-        <v>65</v>
+        <v>310</v>
       </c>
       <c r="G43">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="H43" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I43" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B44" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C44" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D44" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="E44">
-        <v>1205</v>
+        <v>1249.3699999999999</v>
       </c>
       <c r="F44">
-        <v>760</v>
+        <v>240</v>
       </c>
       <c r="G44">
-        <v>270</v>
+        <v>90</v>
       </c>
       <c r="H44" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="I44" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B45" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C45" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D45" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="E45">
-        <v>1844.37</v>
+        <v>1289.3699999999999</v>
       </c>
       <c r="F45">
-        <v>825</v>
+        <v>65</v>
       </c>
       <c r="G45">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="H45" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="I45" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>91</v>
+      </c>
+      <c r="B46" t="s">
         <v>92</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" t="s">
         <v>93</v>
       </c>
-      <c r="C46" t="s">
-        <v>30</v>
-      </c>
-      <c r="D46" t="s">
-        <v>88</v>
-      </c>
       <c r="E46">
-        <v>1579.37</v>
+        <v>1205</v>
       </c>
       <c r="F46">
-        <v>585</v>
+        <v>760</v>
       </c>
       <c r="G46">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="H46" t="s">
         <v>94</v>
@@ -2283,28 +2345,28 @@
         <v>96</v>
       </c>
       <c r="B47" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C47" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D47" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E47">
-        <v>1190</v>
+        <v>1844.37</v>
       </c>
       <c r="F47">
-        <v>1230</v>
+        <v>825</v>
       </c>
       <c r="G47">
         <v>270</v>
       </c>
       <c r="H47" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="I47" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2315,19 +2377,19 @@
         <v>98</v>
       </c>
       <c r="C48" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D48" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E48">
-        <v>1392.2059999999999</v>
+        <v>1579.37</v>
       </c>
       <c r="F48">
-        <v>1363.588</v>
+        <v>585</v>
       </c>
       <c r="G48">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="H48" t="s">
         <v>99</v>
@@ -2341,25 +2403,28 @@
         <v>101</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="C49" t="s">
         <v>20</v>
       </c>
       <c r="D49" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="E49">
-        <v>760</v>
+        <v>1190</v>
       </c>
       <c r="F49">
-        <v>960.59100000000001</v>
+        <v>1230</v>
       </c>
       <c r="G49">
         <v>270</v>
       </c>
       <c r="H49" t="s">
-        <v>59</v>
+        <v>94</v>
+      </c>
+      <c r="I49" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -2367,544 +2432,541 @@
         <v>102</v>
       </c>
       <c r="B50" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="C50" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D50" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="E50">
-        <v>395</v>
+        <v>1392.2059999999999</v>
       </c>
       <c r="F50">
-        <v>566.06700000000001</v>
+        <v>1363.588</v>
       </c>
       <c r="G50">
-        <v>360</v>
+        <v>90</v>
       </c>
       <c r="H50" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="I50" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B51" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="C51" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D51" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="E51">
-        <v>395</v>
+        <v>760</v>
       </c>
       <c r="F51">
-        <v>448.93299999999999</v>
+        <v>960.59100000000001</v>
       </c>
       <c r="G51">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="H51" t="s">
-        <v>75</v>
-      </c>
-      <c r="I51" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B52" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C52" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D52" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E52">
         <v>395</v>
       </c>
       <c r="F52">
-        <v>305</v>
+        <v>566.06700000000001</v>
       </c>
       <c r="G52">
         <v>360</v>
       </c>
       <c r="H52" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I52" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B53" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C53" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D53" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E53">
-        <v>257.46100000000001</v>
+        <v>395</v>
       </c>
       <c r="F53">
-        <v>235</v>
+        <v>448.93299999999999</v>
       </c>
       <c r="G53">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="H53" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I53" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B54" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C54" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D54" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E54">
-        <v>294.86200000000002</v>
+        <v>395</v>
       </c>
       <c r="F54">
-        <v>60</v>
+        <v>305</v>
       </c>
       <c r="G54">
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="H54" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I54" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B55" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C55" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D55" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E55">
-        <v>810</v>
+        <v>257.46100000000001</v>
       </c>
       <c r="F55">
-        <v>566.06700000000001</v>
+        <v>235</v>
       </c>
       <c r="G55">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="H55" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I55" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B56" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C56" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D56" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E56">
-        <v>810</v>
+        <v>294.86200000000002</v>
       </c>
       <c r="F56">
-        <v>448.93299999999999</v>
+        <v>60</v>
       </c>
       <c r="G56">
-        <v>360</v>
+        <v>180</v>
       </c>
       <c r="H56" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I56" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B57" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C57" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D57" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E57">
         <v>810</v>
       </c>
       <c r="F57">
-        <v>305</v>
+        <v>566.06700000000001</v>
       </c>
       <c r="G57">
         <v>180</v>
       </c>
       <c r="H57" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I57" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B58" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C58" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D58" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E58">
-        <v>949.86199999999997</v>
+        <v>810</v>
       </c>
       <c r="F58">
-        <v>235</v>
+        <v>448.93299999999999</v>
       </c>
       <c r="G58">
-        <v>90</v>
+        <v>360</v>
       </c>
       <c r="H58" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I58" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B59" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C59" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D59" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E59">
-        <v>912.46100000000001</v>
+        <v>810</v>
       </c>
       <c r="F59">
-        <v>60</v>
+        <v>305</v>
       </c>
       <c r="G59">
-        <v>360</v>
+        <v>180</v>
       </c>
       <c r="H59" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I59" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="C60" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D60" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E60">
-        <v>600</v>
+        <v>949.86199999999997</v>
       </c>
       <c r="F60">
-        <v>650</v>
+        <v>235</v>
       </c>
       <c r="G60">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="H60" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="I60" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B61" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C61" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D61" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E61">
-        <v>325</v>
+        <v>912.46100000000001</v>
       </c>
       <c r="F61">
-        <v>1365</v>
+        <v>60</v>
       </c>
       <c r="G61">
-        <v>90</v>
+        <v>360</v>
       </c>
       <c r="H61" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="I61" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B62" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="C62" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D62" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="E62">
-        <v>422.20600000000002</v>
+        <v>600</v>
       </c>
       <c r="F62">
-        <v>1366.412</v>
+        <v>650</v>
       </c>
       <c r="G62">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="H62" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="I62" t="s">
-        <v>100</v>
+        <v>73</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B63" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="C63" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D63" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="E63">
-        <v>600</v>
+        <v>325</v>
       </c>
       <c r="F63">
-        <v>565</v>
+        <v>1365</v>
       </c>
       <c r="G63">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="H63" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="I63" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B64" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="C64" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D64" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E64">
-        <v>225</v>
+        <v>422.20600000000002</v>
       </c>
       <c r="F64">
-        <v>760</v>
+        <v>1366.412</v>
       </c>
       <c r="G64">
-        <v>270</v>
+        <v>90</v>
       </c>
       <c r="H64" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="I64" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B65" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C65" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D65" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E65">
-        <v>845</v>
+        <v>600</v>
       </c>
       <c r="F65">
-        <v>825</v>
+        <v>565</v>
       </c>
       <c r="G65">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="H65" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="I65" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B66" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C66" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D66" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E66">
-        <v>2860</v>
+        <v>225</v>
       </c>
       <c r="F66">
-        <v>805</v>
+        <v>760</v>
       </c>
       <c r="G66">
         <v>270</v>
       </c>
       <c r="H66" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="I66" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B67" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C67" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D67" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E67">
-        <v>2235</v>
+        <v>845</v>
       </c>
       <c r="F67">
-        <v>760</v>
+        <v>825</v>
       </c>
       <c r="G67">
         <v>270</v>
       </c>
       <c r="H67" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="I67" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B68" t="s">
+        <v>92</v>
+      </c>
+      <c r="C68" t="s">
+        <v>20</v>
+      </c>
+      <c r="D68" t="s">
         <v>93</v>
       </c>
-      <c r="C68" t="s">
-        <v>30</v>
-      </c>
-      <c r="D68" t="s">
-        <v>88</v>
-      </c>
       <c r="E68">
-        <v>2603.5880000000002</v>
+        <v>2860</v>
       </c>
       <c r="F68">
-        <v>575.53899999999999</v>
+        <v>805</v>
       </c>
       <c r="G68">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="H68" t="s">
         <v>94</v>
@@ -2915,599 +2977,848 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B69" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C69" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D69" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E69">
-        <v>2610</v>
+        <v>2235</v>
       </c>
       <c r="F69">
-        <v>1363.588</v>
+        <v>760</v>
       </c>
       <c r="G69">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="H69" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="I69" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B70" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C70" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D70" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E70">
-        <v>2195</v>
+        <v>2603.5880000000002</v>
       </c>
       <c r="F70">
-        <v>1230</v>
+        <v>575.53899999999999</v>
       </c>
       <c r="G70">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="H70" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="I70" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B71" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
       <c r="C71" t="s">
         <v>20</v>
       </c>
       <c r="D71" t="s">
-        <v>21</v>
+        <v>93</v>
       </c>
       <c r="E71">
-        <v>2595</v>
+        <v>2610</v>
       </c>
       <c r="F71">
-        <v>60</v>
+        <v>1363.588</v>
       </c>
       <c r="G71">
-        <v>360</v>
+        <v>90</v>
       </c>
       <c r="H71" t="s">
-        <v>22</v>
+        <v>104</v>
+      </c>
+      <c r="I71" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B72" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="C72" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D72" t="s">
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="E72">
-        <v>2509.64</v>
+        <v>2195</v>
       </c>
       <c r="F72">
-        <v>1365</v>
+        <v>1230</v>
       </c>
       <c r="G72">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="H72" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="I72" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B73" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="C73" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D73" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="E73">
-        <v>2605</v>
+        <v>2595</v>
       </c>
       <c r="F73">
-        <v>660</v>
+        <v>60</v>
       </c>
       <c r="G73">
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="H73" t="s">
-        <v>67</v>
-      </c>
-      <c r="I73" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B74" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C74" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D74" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E74">
-        <v>2915</v>
+        <v>2509.64</v>
       </c>
       <c r="F74">
-        <v>60</v>
+        <v>1365</v>
       </c>
       <c r="G74">
-        <v>360</v>
+        <v>90</v>
       </c>
       <c r="H74" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I74" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B75" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C75" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D75" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E75">
-        <v>2954.37</v>
+        <v>2605</v>
       </c>
       <c r="F75">
-        <v>215</v>
+        <v>660</v>
       </c>
       <c r="G75">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="H75" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I75" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B76" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C76" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D76" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E76">
-        <v>2820</v>
+        <v>2915</v>
       </c>
       <c r="F76">
-        <v>305</v>
+        <v>60</v>
       </c>
       <c r="G76">
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="H76" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I76" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B77" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C77" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D77" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E77">
-        <v>2820</v>
+        <v>2954.37</v>
       </c>
       <c r="F77">
-        <v>440</v>
+        <v>215</v>
       </c>
       <c r="G77">
-        <v>360</v>
+        <v>90</v>
       </c>
       <c r="H77" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I77" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B78" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C78" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D78" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E78">
         <v>2820</v>
       </c>
       <c r="F78">
-        <v>575</v>
+        <v>305</v>
       </c>
       <c r="G78">
         <v>180</v>
       </c>
       <c r="H78" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I78" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B79" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C79" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D79" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E79">
-        <v>2292.4009999999998</v>
+        <v>2820</v>
       </c>
       <c r="F79">
-        <v>60</v>
+        <v>440</v>
       </c>
       <c r="G79">
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="H79" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I79" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B80" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C80" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D80" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E80">
-        <v>2255</v>
+        <v>2820</v>
       </c>
       <c r="F80">
-        <v>235</v>
+        <v>575</v>
       </c>
       <c r="G80">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="H80" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I80" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B81" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C81" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D81" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E81">
-        <v>2390</v>
+        <v>2292.4009999999998</v>
       </c>
       <c r="F81">
-        <v>305</v>
+        <v>60</v>
       </c>
       <c r="G81">
-        <v>360</v>
+        <v>180</v>
       </c>
       <c r="H81" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I81" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B82" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C82" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D82" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E82">
-        <v>2390</v>
+        <v>2255</v>
       </c>
       <c r="F82">
-        <v>440</v>
+        <v>235</v>
       </c>
       <c r="G82">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="H82" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I82" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B83" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C83" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D83" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E83">
         <v>2390</v>
       </c>
       <c r="F83">
-        <v>575</v>
+        <v>305</v>
       </c>
       <c r="G83">
         <v>360</v>
       </c>
       <c r="H83" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="I83" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B84" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="C84" t="s">
         <v>20</v>
       </c>
       <c r="D84" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E84">
-        <v>2770</v>
+        <v>2390</v>
       </c>
       <c r="F84">
-        <v>960.59100000000001</v>
+        <v>440</v>
       </c>
       <c r="G84">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="H84" t="s">
-        <v>59</v>
+        <v>80</v>
+      </c>
+      <c r="I84" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B85" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="C85" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D85" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E85">
-        <v>2395</v>
+        <v>2390</v>
       </c>
       <c r="F85">
-        <v>979.56700000000001</v>
+        <v>575</v>
       </c>
       <c r="G85">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="H85" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="I85" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B86" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="C86" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D86" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="E86">
-        <v>1574.37</v>
+        <v>2770</v>
       </c>
       <c r="F86">
-        <v>65</v>
+        <v>960.59100000000001</v>
       </c>
       <c r="G86">
-        <v>360</v>
+        <v>270</v>
       </c>
       <c r="H86" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B87" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="C87" t="s">
         <v>20</v>
       </c>
       <c r="D87" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="E87">
-        <v>590</v>
+        <v>2395</v>
       </c>
       <c r="F87">
-        <v>60</v>
+        <v>979.56700000000001</v>
       </c>
       <c r="G87">
-        <v>360</v>
+        <v>0</v>
       </c>
       <c r="H87" t="s">
-        <v>22</v>
+        <v>68</v>
+      </c>
+      <c r="I87" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B88" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="C88" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D88" t="s">
-        <v>88</v>
+        <v>27</v>
       </c>
       <c r="E88">
-        <v>200</v>
+        <v>1574.37</v>
       </c>
       <c r="F88">
-        <v>1230</v>
+        <v>65</v>
       </c>
       <c r="G88">
-        <v>270</v>
+        <v>360</v>
       </c>
       <c r="H88" t="s">
-        <v>89</v>
-      </c>
-      <c r="I88" t="s">
-        <v>90</v>
+        <v>28</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B89" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="C89" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D89" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="E89">
+        <v>590</v>
+      </c>
+      <c r="F89">
+        <v>60</v>
+      </c>
+      <c r="G89">
+        <v>360</v>
+      </c>
+      <c r="H89" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>145</v>
+      </c>
+      <c r="B90" t="s">
+        <v>92</v>
+      </c>
+      <c r="C90" t="s">
+        <v>20</v>
+      </c>
+      <c r="D90" t="s">
+        <v>93</v>
+      </c>
+      <c r="E90">
+        <v>200</v>
+      </c>
+      <c r="F90">
+        <v>1230</v>
+      </c>
+      <c r="G90">
+        <v>270</v>
+      </c>
+      <c r="H90" t="s">
+        <v>94</v>
+      </c>
+      <c r="I90" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>146</v>
+      </c>
+      <c r="B91" t="s">
+        <v>66</v>
+      </c>
+      <c r="C91" t="s">
+        <v>20</v>
+      </c>
+      <c r="D91" t="s">
+        <v>67</v>
+      </c>
+      <c r="E91">
         <v>380</v>
       </c>
-      <c r="F89">
+      <c r="F91">
         <v>979.56700000000001</v>
       </c>
-      <c r="G89">
+      <c r="G91">
         <v>0</v>
       </c>
-      <c r="H89" t="s">
-        <v>63</v>
-      </c>
-      <c r="I89" t="s">
-        <v>64</v>
+      <c r="H91" t="s">
+        <v>68</v>
+      </c>
+      <c r="I91" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>147</v>
+      </c>
+      <c r="B92" t="s">
+        <v>148</v>
+      </c>
+      <c r="C92" t="s">
+        <v>20</v>
+      </c>
+      <c r="D92" t="s">
+        <v>50</v>
+      </c>
+      <c r="E92">
+        <v>2860</v>
+      </c>
+      <c r="F92">
+        <v>2710</v>
+      </c>
+      <c r="G92">
+        <v>90</v>
+      </c>
+      <c r="H92" t="s">
+        <v>149</v>
+      </c>
+      <c r="I92" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>151</v>
+      </c>
+      <c r="B93" t="s">
+        <v>148</v>
+      </c>
+      <c r="C93" t="s">
+        <v>20</v>
+      </c>
+      <c r="D93" t="s">
+        <v>50</v>
+      </c>
+      <c r="E93">
+        <v>2770</v>
+      </c>
+      <c r="F93">
+        <v>2710</v>
+      </c>
+      <c r="G93">
+        <v>90</v>
+      </c>
+      <c r="H93" t="s">
+        <v>149</v>
+      </c>
+      <c r="I93" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>152</v>
+      </c>
+      <c r="B94" t="s">
+        <v>153</v>
+      </c>
+      <c r="C94" t="s">
+        <v>26</v>
+      </c>
+      <c r="D94" t="s">
+        <v>154</v>
+      </c>
+      <c r="E94">
+        <v>2680</v>
+      </c>
+      <c r="F94">
+        <v>3090</v>
+      </c>
+      <c r="G94">
+        <v>90</v>
+      </c>
+      <c r="H94" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>156</v>
+      </c>
+      <c r="B95" t="s">
+        <v>25</v>
+      </c>
+      <c r="C95" t="s">
+        <v>26</v>
+      </c>
+      <c r="D95" t="s">
+        <v>27</v>
+      </c>
+      <c r="E95">
+        <v>2775</v>
+      </c>
+      <c r="F95">
+        <v>3735</v>
+      </c>
+      <c r="G95">
+        <v>180</v>
+      </c>
+      <c r="H95" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>157</v>
+      </c>
+      <c r="B96" t="s">
+        <v>158</v>
+      </c>
+      <c r="C96" t="s">
+        <v>20</v>
+      </c>
+      <c r="D96" t="s">
+        <v>159</v>
+      </c>
+      <c r="E96">
+        <v>2510</v>
+      </c>
+      <c r="F96">
+        <v>2615</v>
+      </c>
+      <c r="G96">
+        <v>270</v>
+      </c>
+      <c r="H96" t="s">
+        <v>160</v>
+      </c>
+      <c r="I96" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>162</v>
+      </c>
+      <c r="B97" t="s">
+        <v>153</v>
+      </c>
+      <c r="C97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D97" t="s">
+        <v>154</v>
+      </c>
+      <c r="E97">
+        <v>2945</v>
+      </c>
+      <c r="F97">
+        <v>3090</v>
+      </c>
+      <c r="G97">
+        <v>90</v>
+      </c>
+      <c r="H97" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>163</v>
+      </c>
+      <c r="B98" t="s">
+        <v>25</v>
+      </c>
+      <c r="C98" t="s">
+        <v>26</v>
+      </c>
+      <c r="D98" t="s">
+        <v>27</v>
+      </c>
+      <c r="E98">
+        <v>3225</v>
+      </c>
+      <c r="F98">
+        <v>3735</v>
+      </c>
+      <c r="G98">
+        <v>180</v>
+      </c>
+      <c r="H98" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>